<commit_message>
init project for deployment
</commit_message>
<xml_diff>
--- a/data/operation_rates.xlsx
+++ b/data/operation_rates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturdavydov/Desktop/WEBIA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturdavydov/Desktop/BU/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F0874-C3D8-454E-A97A-4777E25B443F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A70C0A-D580-D547-9485-9D58403D21FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{7DBD2ACD-B6E5-ED45-9D38-D5BC44582964}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="19200" xr2:uid="{7DBD2ACD-B6E5-ED45-9D38-D5BC44582964}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -394,12 +394,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -414,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,6 +429,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -739,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D5054D-8171-A144-8A4C-F8CC81491318}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="75" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,31 +954,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D15" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="9">
         <v>14</v>
       </c>
     </row>
@@ -1155,31 +1164,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D30" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="9">
         <v>14</v>
       </c>
     </row>
@@ -1337,31 +1346,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B43" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="D43" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B44" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="10">
         <v>14</v>
       </c>
     </row>
@@ -1757,31 +1766,31 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="73" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B73" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B73" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="10">
         <v>5.5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="74" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B74" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D74" s="10">
         <v>5.5</v>
       </c>
     </row>
@@ -1911,31 +1920,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="84" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B84" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="B84" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D84" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="85" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B85" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="B85" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D85" s="10">
         <v>5</v>
       </c>
     </row>

</xml_diff>